<commit_message>
Initial commit to AIG repo
</commit_message>
<xml_diff>
--- a/Excel_Test_Data/Inventory_Test_Data.xlsx
+++ b/Excel_Test_Data/Inventory_Test_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Direct_Receipt_Medicines" sheetId="3" r:id="rId3"/>
     <sheet name="Adjustments" sheetId="5" r:id="rId4"/>
     <sheet name="Item_Mapping" sheetId="6" r:id="rId5"/>
+    <sheet name="Indent_Items" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Item_Mapping!$A$1:$A$2</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>FieldName</t>
   </si>
@@ -176,6 +177,12 @@
   </si>
   <si>
     <t>ZYROP 5000 IU INJ</t>
+  </si>
+  <si>
+    <t>Indent Items</t>
+  </si>
+  <si>
+    <t>Search_Option</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -2562,4 +2569,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>